<commit_message>
Lab 8 TB bugs
</commit_message>
<xml_diff>
--- a/DE1_SoC_Lab8/doc/FilterCoeffCalc.xlsx
+++ b/DE1_SoC_Lab8/doc/FilterCoeffCalc.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="S:\CPET_561_GIT\DE1_SoC_Lab8\doc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{791EB682-200E-4C1C-A9C5-01B47F08AA55}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{186FAF4A-846E-4AF9-8BB7-7CFF424364BA}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12225" xr2:uid="{D1B6497E-7CA4-4F30-82AE-42CE3C8F9EFA}"/>
   </bookViews>
@@ -142,13 +142,13 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="2" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -467,8 +467,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AB888FB4-A5EF-430F-952A-F0EFA2811C1F}">
   <dimension ref="A1:G19"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="190" zoomScaleNormal="190" workbookViewId="0">
+      <selection activeCell="E12" sqref="E12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -481,14 +481,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B1" s="2" t="s">
+      <c r="B1" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="2"/>
-      <c r="D1" s="2" t="s">
+      <c r="C1" s="4"/>
+      <c r="D1" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="E1" s="2"/>
+      <c r="E1" s="4"/>
       <c r="G1" t="s">
         <v>22</v>
       </c>
@@ -520,14 +520,14 @@
       <c r="B3">
         <v>2.5000000000000001E-3</v>
       </c>
-      <c r="C3" s="3" t="str">
+      <c r="C3" s="2" t="str">
         <f>DEC2HEX(INT(B3*2^G2))</f>
         <v>51</v>
       </c>
       <c r="D3">
         <v>1.9E-3</v>
       </c>
-      <c r="E3" s="3" t="str">
+      <c r="E3" s="2" t="str">
         <f>DEC2HEX(INT(D3*2^G2))</f>
         <v>3E</v>
       </c>
@@ -539,16 +539,16 @@
       <c r="B4">
         <v>5.7000000000000002E-3</v>
       </c>
-      <c r="C4" s="3" t="str">
+      <c r="C4" s="2" t="str">
         <f>DEC2HEX(INT(B4*2^G2))</f>
         <v>BA</v>
       </c>
       <c r="D4">
-        <v>3.0999999999999999E-3</v>
-      </c>
-      <c r="E4" s="3" t="str">
+        <v>-3.0999999999999999E-3</v>
+      </c>
+      <c r="E4" s="2" t="str">
         <f>DEC2HEX(INT(D4*2^G2))</f>
-        <v>65</v>
+        <v>FFFFFFFF9A</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
@@ -558,14 +558,14 @@
       <c r="B5">
         <v>1.47E-2</v>
       </c>
-      <c r="C5" s="3" t="str">
+      <c r="C5" s="2" t="str">
         <f>DEC2HEX(INT(B5*2^G2))</f>
         <v>1E1</v>
       </c>
       <c r="D5">
-        <v>1.0800000000000001E-2</v>
-      </c>
-      <c r="E5" s="3" t="str">
+        <v>-1.0800000000000001E-2</v>
+      </c>
+      <c r="E5" s="2" t="str">
         <f>DEC2HEX(INT(D6*2^G2))</f>
         <v>0</v>
       </c>
@@ -577,14 +577,14 @@
       <c r="B6">
         <v>3.15E-2</v>
       </c>
-      <c r="C6" s="3" t="str">
+      <c r="C6" s="2" t="str">
         <f>DEC2HEX(INT(B6*2^G2))</f>
         <v>408</v>
       </c>
       <c r="D6">
         <v>0</v>
       </c>
-      <c r="E6" s="3" t="str">
+      <c r="E6" s="2" t="str">
         <f>DEC2HEX(INT(D6*2^G2))</f>
         <v>0</v>
       </c>
@@ -596,14 +596,14 @@
       <c r="B7">
         <v>5.5500000000000001E-2</v>
       </c>
-      <c r="C7" s="3" t="str">
+      <c r="C7" s="2" t="str">
         <f>DEC2HEX(INT(B7*2^G2))</f>
         <v>71A</v>
       </c>
       <c r="D7">
         <v>4.07E-2</v>
       </c>
-      <c r="E7" s="3" t="str">
+      <c r="E7" s="2" t="str">
         <f>DEC2HEX(INT(D7*2^G2))</f>
         <v>535</v>
       </c>
@@ -615,14 +615,14 @@
       <c r="B8">
         <v>8.3400000000000002E-2</v>
       </c>
-      <c r="C8" s="3" t="str">
+      <c r="C8" s="2" t="str">
         <f>DEC2HEX(INT(B8*2^G2))</f>
         <v>AAC</v>
       </c>
       <c r="D8">
         <v>4.4499999999999998E-2</v>
       </c>
-      <c r="E8" s="3" t="str">
+      <c r="E8" s="2" t="str">
         <f>DEC2HEX(INT(D8*2^G2))</f>
         <v>5B2</v>
       </c>
@@ -634,16 +634,16 @@
       <c r="B9">
         <v>0.1099</v>
       </c>
-      <c r="C9" s="3" t="str">
+      <c r="C9" s="2" t="str">
         <f>DEC2HEX(INT(B9*2^G2))</f>
         <v>E11</v>
       </c>
       <c r="D9">
-        <v>8.0699999999999994E-2</v>
-      </c>
-      <c r="E9" s="3" t="str">
+        <v>-8.0699999999999994E-2</v>
+      </c>
+      <c r="E9" s="2" t="str">
         <f>DEC2HEX(INT(D9*2^G2))</f>
-        <v>A54</v>
+        <v>FFFFFFF5AB</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
@@ -653,16 +653,16 @@
       <c r="B10">
         <v>0.12889999999999999</v>
       </c>
-      <c r="C10" s="4" t="str">
+      <c r="C10" s="3" t="str">
         <f>DEC2HEX(INT(B10*2^G2))</f>
         <v>107F</v>
       </c>
       <c r="D10">
-        <v>0.2913</v>
-      </c>
-      <c r="E10" s="3" t="str">
+        <v>-0.2913</v>
+      </c>
+      <c r="E10" s="2" t="str">
         <f>DEC2HEX(INT(D10*2^G2))</f>
-        <v>2549</v>
+        <v>FFFFFFDAB6</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
@@ -672,14 +672,14 @@
       <c r="B11">
         <v>0.1358</v>
       </c>
-      <c r="C11" s="3" t="str">
+      <c r="C11" s="2" t="str">
         <f>DEC2HEX(INT(B11*2^G2))</f>
         <v>1161</v>
       </c>
       <c r="D11">
         <v>0.59819999999999995</v>
       </c>
-      <c r="E11" s="3" t="str">
+      <c r="E11" s="2" t="str">
         <f>DEC2HEX(INT(D11*2^G2))</f>
         <v>4C91</v>
       </c>
@@ -691,12 +691,12 @@
       <c r="B12">
         <v>0.12889999999999999</v>
       </c>
-      <c r="C12" s="3" t="str">
+      <c r="C12" s="2" t="str">
         <f>DEC2HEX(INT(B12*2^G2))</f>
         <v>107F</v>
       </c>
       <c r="D12">
-        <v>0.2913</v>
+        <v>-0.2913</v>
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.25">
@@ -706,12 +706,12 @@
       <c r="B13">
         <v>0.1099</v>
       </c>
-      <c r="C13" s="3" t="str">
+      <c r="C13" s="2" t="str">
         <f>DEC2HEX(INT(B13*2^G2))</f>
         <v>E11</v>
       </c>
       <c r="D13">
-        <v>8.0699999999999994E-2</v>
+        <v>-8.0699999999999994E-2</v>
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.25">
@@ -721,7 +721,7 @@
       <c r="B14">
         <v>8.3400000000000002E-2</v>
       </c>
-      <c r="C14" s="3" t="str">
+      <c r="C14" s="2" t="str">
         <f>DEC2HEX(INT(B14*2^G2))</f>
         <v>AAC</v>
       </c>
@@ -736,7 +736,7 @@
       <c r="B15">
         <v>5.5500000000000001E-2</v>
       </c>
-      <c r="C15" s="3" t="str">
+      <c r="C15" s="2" t="str">
         <f>DEC2HEX(INT(B7*2^G2))</f>
         <v>71A</v>
       </c>
@@ -751,7 +751,7 @@
       <c r="B16">
         <v>3.15E-2</v>
       </c>
-      <c r="C16" s="3" t="str">
+      <c r="C16" s="2" t="str">
         <f>DEC2HEX(INT(B16*2^G2))</f>
         <v>408</v>
       </c>
@@ -766,12 +766,12 @@
       <c r="B17">
         <v>1.47E-2</v>
       </c>
-      <c r="C17" s="3" t="str">
+      <c r="C17" s="2" t="str">
         <f>DEC2HEX(INT(B17*2^G2))</f>
         <v>1E1</v>
       </c>
       <c r="D17">
-        <v>1.0800000000000001E-2</v>
+        <v>-1.0800000000000001E-2</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
@@ -781,12 +781,12 @@
       <c r="B18">
         <v>5.7000000000000002E-3</v>
       </c>
-      <c r="C18" s="3" t="str">
+      <c r="C18" s="2" t="str">
         <f>DEC2HEX(INT(B18*2^G2))</f>
         <v>BA</v>
       </c>
       <c r="D18">
-        <v>3.0999999999999999E-3</v>
+        <v>-3.0999999999999999E-3</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.25">
@@ -796,7 +796,7 @@
       <c r="B19">
         <v>2.5000000000000001E-3</v>
       </c>
-      <c r="C19" s="3" t="str">
+      <c r="C19" s="2" t="str">
         <f>DEC2HEX(INT(B19*2^G2))</f>
         <v>51</v>
       </c>

</xml_diff>

<commit_message>
Finished lab 8 and tested it.
</commit_message>
<xml_diff>
--- a/DE1_SoC_Lab8/doc/FilterCoeffCalc.xlsx
+++ b/DE1_SoC_Lab8/doc/FilterCoeffCalc.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20391"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25726"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="S:\CPET_561_GIT\DE1_SoC_Lab8\doc\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\CPET_561_GIT\DE1_SoC_Lab8\doc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{186FAF4A-846E-4AF9-8BB7-7CFF424364BA}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8D6F4E00-66FF-4F99-8C41-057F4AC89D51}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12225" xr2:uid="{D1B6497E-7CA4-4F30-82AE-42CE3C8F9EFA}"/>
+    <workbookView xWindow="336" yWindow="2748" windowWidth="21600" windowHeight="11268" xr2:uid="{D1B6497E-7CA4-4F30-82AE-42CE3C8F9EFA}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -19,6 +19,17 @@
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
@@ -467,20 +478,20 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AB888FB4-A5EF-430F-952A-F0EFA2811C1F}">
   <dimension ref="A1:G19"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="190" zoomScaleNormal="190" workbookViewId="0">
-      <selection activeCell="E12" sqref="E12"/>
+    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="E19" sqref="E19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
   <cols>
     <col min="1" max="1" width="13" customWidth="1"/>
-    <col min="2" max="2" width="9.7109375" customWidth="1"/>
+    <col min="2" max="2" width="9.68359375" customWidth="1"/>
     <col min="3" max="3" width="16" customWidth="1"/>
-    <col min="5" max="5" width="16.140625" customWidth="1"/>
-    <col min="7" max="7" width="21.140625" customWidth="1"/>
+    <col min="5" max="5" width="16.15625" customWidth="1"/>
+    <col min="7" max="7" width="21.15625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="B1" s="4" t="s">
         <v>1</v>
       </c>
@@ -493,7 +504,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -513,7 +524,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A3" t="s">
         <v>5</v>
       </c>
@@ -532,7 +543,7 @@
         <v>3E</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A4" t="s">
         <v>6</v>
       </c>
@@ -551,7 +562,7 @@
         <v>FFFFFFFF9A</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A5" t="s">
         <v>7</v>
       </c>
@@ -566,11 +577,11 @@
         <v>-1.0800000000000001E-2</v>
       </c>
       <c r="E5" s="2" t="str">
-        <f>DEC2HEX(INT(D6*2^G2))</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+        <f>DEC2HEX(INT(D5*2^G2))</f>
+        <v>FFFFFFFE9E</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A6" t="s">
         <v>8</v>
       </c>
@@ -589,7 +600,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A7" t="s">
         <v>9</v>
       </c>
@@ -608,7 +619,7 @@
         <v>535</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A8" t="s">
         <v>10</v>
       </c>
@@ -627,7 +638,7 @@
         <v>5B2</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A9" t="s">
         <v>11</v>
       </c>
@@ -646,7 +657,7 @@
         <v>FFFFFFF5AB</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A10" t="s">
         <v>12</v>
       </c>
@@ -665,7 +676,7 @@
         <v>FFFFFFDAB6</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A11" t="s">
         <v>13</v>
       </c>
@@ -684,7 +695,7 @@
         <v>4C91</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A12" t="s">
         <v>14</v>
       </c>
@@ -699,7 +710,7 @@
         <v>-0.2913</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A13" t="s">
         <v>15</v>
       </c>
@@ -714,7 +725,7 @@
         <v>-8.0699999999999994E-2</v>
       </c>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A14" t="s">
         <v>16</v>
       </c>
@@ -729,7 +740,7 @@
         <v>4.4499999999999998E-2</v>
       </c>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A15" t="s">
         <v>17</v>
       </c>
@@ -744,7 +755,7 @@
         <v>4.07E-2</v>
       </c>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A16" t="s">
         <v>18</v>
       </c>
@@ -759,7 +770,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A17" t="s">
         <v>19</v>
       </c>
@@ -774,7 +785,7 @@
         <v>-1.0800000000000001E-2</v>
       </c>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A18" t="s">
         <v>20</v>
       </c>
@@ -789,7 +800,7 @@
         <v>-3.0999999999999999E-3</v>
       </c>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A19" t="s">
         <v>21</v>
       </c>

</xml_diff>